<commit_message>
Listing users, towns and categories
Listing users, towns and categories
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1107,7 +1107,9 @@
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="7"/>
+      <c r="E37" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
@@ -1117,7 +1119,9 @@
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="7"/>
+      <c r="E38" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
@@ -1127,7 +1131,9 @@
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
@@ -1167,7 +1173,9 @@
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
@@ -1207,7 +1215,9 @@
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E47" s="7"/>
+      <c r="E47" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
@@ -1245,7 +1255,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Creating towns and categories
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1185,7 +1185,9 @@
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
@@ -1195,7 +1197,9 @@
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
@@ -1205,7 +1209,9 @@
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
@@ -1227,7 +1233,9 @@
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -1237,7 +1245,9 @@
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
@@ -1247,7 +1257,9 @@
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="51" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
@@ -1255,7 +1267,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>